<commit_message>
Render first line chart with EWLD ETF
</commit_message>
<xml_diff>
--- a/apps/frontend/src/assets/Historique des VLs_Lyxor PEA Monde (MSCI World) UCITS ETF - Capi._FR0011869353_13_05_2014.xlsx
+++ b/apps/frontend/src/assets/Historique des VLs_Lyxor PEA Monde (MSCI World) UCITS ETF - Capi._FR0011869353_13_05_2014.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B602AD4-A382-AA45-9D77-A8D68C9B95B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C655B52-BE02-C54A-90B4-290D1A7C4A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16798,8 +16798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2476"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2447" workbookViewId="0">
+      <selection activeCell="A2471" sqref="A41:XFD2471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -51240,27 +51240,27 @@
       <c r="B2473" s="10" t="s">
         <v>5427</v>
       </c>
-      <c r="C2473" s="7"/>
-      <c r="D2473" s="7"/>
-      <c r="E2473" s="7"/>
+      <c r="C2473" s="10"/>
+      <c r="D2473" s="10"/>
+      <c r="E2473" s="10"/>
     </row>
     <row r="2475" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2475" s="1"/>
       <c r="B2475" s="10" t="s">
         <v>5428</v>
       </c>
-      <c r="C2475" s="7"/>
-      <c r="D2475" s="7"/>
-      <c r="E2475" s="7"/>
+      <c r="C2475" s="10"/>
+      <c r="D2475" s="10"/>
+      <c r="E2475" s="10"/>
     </row>
     <row r="2476" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2476" s="1"/>
       <c r="B2476" s="10" t="s">
         <v>5429</v>
       </c>
-      <c r="C2476" s="7"/>
-      <c r="D2476" s="7"/>
-      <c r="E2476" s="7"/>
+      <c r="C2476" s="10"/>
+      <c r="D2476" s="10"/>
+      <c r="E2476" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>